<commit_message>
Update Gantt chart and Project Plan
</commit_message>
<xml_diff>
--- a/ASM_PartA/Gantt chart.xlsx
+++ b/ASM_PartA/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunwoonam/Desktop/Griffith/2023_T2/7810_Software Technologies/Assessment/Stage1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E26FB9C-4FB2-3B48-BC37-D9A587F126CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B50A44-60F8-7B44-B531-988E49BEC711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -622,12 +622,27 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -648,21 +663,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -830,6 +830,19 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
@@ -892,19 +905,6 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
         </patternFill>
       </fill>
       <border>
@@ -1179,8 +1179,8 @@
   </sheetPr>
   <dimension ref="B1:BO27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AM11" sqref="AM11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="CC6" sqref="CC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1189,13 +1189,14 @@
     <col min="2" max="2" width="47.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="14" width="2.83203125" style="1"/>
     <col min="15" max="15" width="2.83203125" style="1" customWidth="1"/>
     <col min="16" max="27" width="2.83203125" style="1"/>
     <col min="42" max="42" width="2.83203125" customWidth="1"/>
+    <col min="71" max="71" width="4.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
@@ -1209,13 +1210,13 @@
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1223,37 +1224,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="35"/>
       <c r="P2" s="16"/>
-      <c r="Q2" s="28" t="s">
+      <c r="Q2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="30"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="35"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="32" t="s">
+      <c r="V2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="34"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="39"/>
       <c r="Z2" s="18"/>
-      <c r="AA2" s="32" t="s">
+      <c r="AA2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="34"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="39"/>
       <c r="AH2" s="19"/>
       <c r="AI2" s="21" t="s">
         <v>4</v>
@@ -1267,22 +1268,22 @@
       <c r="AP2" s="22"/>
     </row>
     <row r="3" spans="2:67" s="11" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="38" t="s">
+      <c r="B3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="32" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="20" t="s">
@@ -1309,12 +1310,12 @@
       <c r="AA3" s="10"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1588,7 +1589,7 @@
         <v>1</v>
       </c>
       <c r="Q8" s="17"/>
-      <c r="R8" s="39"/>
+      <c r="R8" s="26"/>
       <c r="AB8" s="1"/>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1992,17 +1993,17 @@
     <row r="27" spans="2:67" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="16" priority="8">
@@ -2010,23 +2011,23 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5:BO5 H6:M6 Q6:BO6 R7:BO7 H7:O26">
-    <cfRule type="expression" dxfId="15" priority="1">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="1">
+      <formula>PercentComplete</formula>
     </cfRule>
     <cfRule type="expression" dxfId="9" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
@@ -2035,7 +2036,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8:BO8 Q9 U9:BO9 Q10:R10 V10:BO10 Q11:S11 U11 W11:BO11 Q12:T12 V12 X12:BO12 Q13:U13 AB13:BO13 Q14:Y14 AE14:BO14 Q15:AB15 AH15:BO15 Q16:AD16 AG16 AJ16:BO16 Q17:AI17 AN17:BO17 Q18:AM18 AR18:BO18 Q19:AQ19 AU19:BO19 Q20:AT20 AX20:BO20 Q21:AW21 BE21:BO21 Q22:BD22 BG22:BO22 Q23:BF23 BI23:BO23 Q24:BH24 BK24:BO24 Q25:BJ25 BN25:BO25 Q26:BM26 T10">
+  <conditionalFormatting sqref="S8:BO8 Q9 U9:BO9 Q10:R10 T10 V10:BO10 Q11:S11 U11 W11:BO11 Q12:T12 V12 X12:BO12 Q13:U13 AB13:BO13 Q14:Y14 AE14:BO14 Q15:AB15 AH15:BO15 Q16:AD16 AG16 AJ16:BO16 Q17:AI17 AN17:BO17 Q18:AM18 AR18:BO18 Q19:AQ19 AU19:BO19 Q20:AT20 AX20:BO20 Q21:AW21 BE21:BO21 Q22:BD22 BG22:BO22 Q23:BF23 BI23:BO23 Q24:BH24 BK24:BO24 Q25:BJ25 BN25:BO25 Q26:BM26">
     <cfRule type="expression" dxfId="7" priority="21">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>